<commit_message>
Fixing plasma all to plasma AngII
</commit_message>
<xml_diff>
--- a/35_Mr_Parks/Mr_Parks_Data.xlsx
+++ b/35_Mr_Parks/Mr_Parks_Data.xlsx
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>Renal Autonomic Firing Rate</t>
-  </si>
-  <si>
-    <t>Plasma [AII]</t>
   </si>
   <si>
     <t>pG/mL</t>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>30 Days</t>
+  </si>
+  <si>
+    <t>Plasma [AngII]</t>
   </si>
 </sst>
 </file>
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51:D55"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -952,7 +952,7 @@
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1">
       <c r="A30" s="3" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="B30" s="4">
         <v>50</v>
@@ -961,7 +961,7 @@
         <v>20</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1"/>
@@ -981,7 +981,7 @@
     </row>
     <row r="33" spans="1:5" ht="30.75" thickBot="1">
       <c r="A33" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="4">
         <v>0</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="34" spans="1:5" ht="30.75" thickBot="1">
       <c r="A34" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="4">
         <v>0</v>
@@ -1013,16 +1013,16 @@
         <v>0</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30.75" thickBot="1">
@@ -1033,13 +1033,13 @@
         <v>5</v>
       </c>
       <c r="C37" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>43</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1">
@@ -1146,7 +1146,7 @@
     </row>
     <row r="44" spans="1:5" ht="35.25" thickBot="1">
       <c r="A44" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44" s="5">
         <v>0.19</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="45" spans="1:5" ht="35.25" thickBot="1">
       <c r="A45" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="5">
         <v>0.12</v>
@@ -1184,10 +1184,10 @@
         <v>0</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>3</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="48" spans="1:5" ht="30.75" thickBot="1">
       <c r="A48" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48" s="4">
         <v>1.4E-2</v>
@@ -1204,12 +1204,12 @@
         <v>0.114</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30.75" thickBot="1">
       <c r="A49" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B49" s="4">
         <v>0.2</v>
@@ -1227,10 +1227,10 @@
         <v>0</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Fixing Brain/Hepatic Vein Data in Lab 35
</commit_message>
<xml_diff>
--- a/35_Mr_Parks/Mr_Parks_Data.xlsx
+++ b/35_Mr_Parks/Mr_Parks_Data.xlsx
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -984,7 +984,7 @@
         <v>35</v>
       </c>
       <c r="B33" s="4">
-        <v>0</v>
+        <v>648</v>
       </c>
       <c r="C33" s="4">
         <v>706</v>
@@ -998,7 +998,7 @@
         <v>36</v>
       </c>
       <c r="B34" s="4">
-        <v>0</v>
+        <v>553</v>
       </c>
       <c r="C34" s="4">
         <v>1217</v>

</xml_diff>